<commit_message>
Actualizacion medicion y monitoreo
</commit_message>
<xml_diff>
--- a/Organizacional/06. Medición y Monitoreo/2016/Bisoltec-ConcentradoMetricas.xlsx
+++ b/Organizacional/06. Medición y Monitoreo/2016/Bisoltec-ConcentradoMetricas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ObjetivosNegocio" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,10 @@
     <sheet name="O4-M3" sheetId="6" state="hidden" r:id="rId7"/>
     <sheet name="M9 - Proyectos" sheetId="7" state="hidden" r:id="rId8"/>
     <sheet name="M6 - Avance de Procesos" sheetId="8" state="hidden" r:id="rId9"/>
+    <sheet name="Apego a Productos" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Apego a Procesos" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Físicas" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Funcionales" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -52,6 +56,42 @@
             <charset val="1"/>
           </rPr>
           <t>Nombre de la medición que ayuda a satisfacer el objetivo</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>.:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Preguntas referente a todos los documentos, verificar que coincidan con lo estimado y planeado.</t>
         </r>
       </text>
     </comment>
@@ -606,7 +646,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="122">
   <si>
     <t>Objetivos de Negocio</t>
   </si>
@@ -899,6 +939,84 @@
 ¿Qué desviacion tubo la proyeccion de proyecto?
 </t>
   </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Productos de Proceso</t>
+  </si>
+  <si>
+    <t>Análisis de Requerimientos</t>
+  </si>
+  <si>
+    <t>Estimación</t>
+  </si>
+  <si>
+    <t>Propuesta</t>
+  </si>
+  <si>
+    <t>Plan de proyecto</t>
+  </si>
+  <si>
+    <t>Plan de Pruebas</t>
+  </si>
+  <si>
+    <t>Carta de Aceptación</t>
+  </si>
+  <si>
+    <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>Productos Organizacionales</t>
+  </si>
+  <si>
+    <t>Plan de Calidad</t>
+  </si>
+  <si>
+    <t>Cronograma</t>
+  </si>
+  <si>
+    <t>Plan de Configuración</t>
+  </si>
+  <si>
+    <t>Plan de Métricas</t>
+  </si>
+  <si>
+    <t>Procesos de procesos</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Medición y Monitoreo</t>
+  </si>
+  <si>
+    <t>Procesos Organizacionales</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t>Elementos de Configuración</t>
+  </si>
+  <si>
+    <t>Línea Base</t>
+  </si>
+  <si>
+    <t>Control de Cambios</t>
+  </si>
+  <si>
+    <t>Líneas Base</t>
+  </si>
+  <si>
+    <t>Entregables</t>
+  </si>
 </sst>
 </file>
 
@@ -908,7 +1026,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="[$$-80A]#,##0.00;[RED]\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
-    <numFmt numFmtId="167" formatCode="GENERAL"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1007,11 +1125,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1054,19 +1167,29 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="16"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1100,7 +1223,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1118,7 +1241,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1127,8 +1250,20 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1332,6 +1467,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="dotted">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1358,7 +1506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="100">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1563,11 +1711,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1575,11 +1723,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1587,67 +1735,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1655,39 +1803,39 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="8" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1695,12 +1843,68 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1733,7 +1937,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF376092"/>
@@ -1779,26 +1983,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Desviación Costos</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1838,6 +2022,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1900,11 +2085,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="95955761"/>
-        <c:axId val="28165233"/>
+        <c:axId val="83828064"/>
+        <c:axId val="36328414"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95955761"/>
+        <c:axId val="83828064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1920,14 +2105,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28165233"/>
+        <c:crossAx val="36328414"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28165233"/>
+        <c:axId val="36328414"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1952,7 +2137,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95955761"/>
+        <c:crossAx val="83828064"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1991,26 +2176,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Costos generales de proyectos</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2039,6 +2204,7 @@
             </a:ln>
           </c:spPr>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2110,6 +2276,7 @@
             </a:ln>
           </c:spPr>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2160,11 +2327,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="95319780"/>
-        <c:axId val="52404150"/>
+        <c:axId val="65317355"/>
+        <c:axId val="60586943"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95319780"/>
+        <c:axId val="65317355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2180,14 +2347,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="52404150"/>
+        <c:crossAx val="60586943"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52404150"/>
+        <c:axId val="60586943"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2212,7 +2379,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95319780"/>
+        <c:crossAx val="65317355"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2251,29 +2418,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1600">
-                <a:solidFill>
-                  <a:srgbClr val="404040"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Apego a Procesos</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2707,11 +2851,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="67028298"/>
-        <c:axId val="87442097"/>
+        <c:axId val="99477288"/>
+        <c:axId val="23892365"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67028298"/>
+        <c:axId val="99477288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,14 +2872,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87442097"/>
+        <c:crossAx val="23892365"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87442097"/>
+        <c:axId val="23892365"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2761,7 +2905,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="67028298"/>
+        <c:crossAx val="99477288"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="20"/>
       </c:valAx>
@@ -2804,29 +2948,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1600">
-                <a:solidFill>
-                  <a:srgbClr val="404040"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Apego a Productos de Trabajo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3260,11 +3381,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="65647417"/>
-        <c:axId val="12768848"/>
+        <c:axId val="5376323"/>
+        <c:axId val="81829371"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65647417"/>
+        <c:axId val="5376323"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3281,14 +3402,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="12768848"/>
+        <c:crossAx val="81829371"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12768848"/>
+        <c:axId val="81829371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3314,7 +3435,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65647417"/>
+        <c:crossAx val="5376323"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="20"/>
       </c:valAx>
@@ -3357,29 +3478,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" sz="1600">
-                <a:solidFill>
-                  <a:srgbClr val="404040"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Número de No Conformidades</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3813,11 +3911,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="62555199"/>
-        <c:axId val="55524384"/>
+        <c:axId val="37411631"/>
+        <c:axId val="61244609"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="62555199"/>
+        <c:axId val="37411631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,14 +3932,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55524384"/>
+        <c:crossAx val="61244609"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55524384"/>
+        <c:axId val="61244609"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -3867,7 +3965,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62555199"/>
+        <c:crossAx val="37411631"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
@@ -3907,30 +4005,1042 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Apego a Productos'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Productos de Proceso</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Apego a Productos'!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Análisis de Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Estimación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Propuesta</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Plan de proyecto</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Plan de Pruebas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Carta de Aceptación</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Reporte de Monitoreo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Apego a Productos'!$J$3:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89205</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="93939710"/>
+        <c:axId val="82642994"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93939710"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="82642994"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="82642994"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="93939710"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Apego a Productos'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Productos Organizacionales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Apego a Productos'!$A$18:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Plan de Calidad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cronograma</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Plan de Configuración</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Plan de Métricas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Apego a Productos'!$J$18:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8889</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="26986985"/>
+        <c:axId val="97004135"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="26986985"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="97004135"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="97004135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="26986985"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Apego a Procesos'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Procesos de procesos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Apego a Procesos'!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Medición y Monitoreo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Apego a Procesos'!$J$3:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="58220877"/>
+        <c:axId val="7967289"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="58220877"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="7967289"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7967289"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="58220877"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Apego a Procesos'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Procesos Organizacionales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Apego a Procesos'!$A$12:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Calidad</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Medición y Monitoreo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Apego a Procesos'!$J$12:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="98417882"/>
+        <c:axId val="55892139"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98417882"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="55892139"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="55892139"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="98417882"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Físicas!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Física</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Físicas!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Elementos de Configuración</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Línea Base</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Control de Cambios</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Físicas!$J$3:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="16247257"/>
+        <c:axId val="62041695"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="16247257"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="62041695"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="62041695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="16247257"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Funcionales!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Funcional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Funcionales!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Líneas Base</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Entregables</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Control de Cambios</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Funcionales!$J$3:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="99643929"/>
+        <c:axId val="91092842"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="99643929"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="91092842"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="91092842"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="99643929"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Desviación de Esfuerzo</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3970,6 +5080,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4032,11 +5143,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="73065338"/>
-        <c:axId val="47019651"/>
+        <c:axId val="84678169"/>
+        <c:axId val="52591298"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73065338"/>
+        <c:axId val="84678169"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4052,14 +5163,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47019651"/>
+        <c:crossAx val="52591298"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47019651"/>
+        <c:axId val="52591298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4084,7 +5195,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73065338"/>
+        <c:crossAx val="84678169"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4123,26 +5234,6 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Esfuerzo en Horas totales</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -4171,6 +5262,7 @@
             </a:ln>
           </c:spPr>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4242,6 +5334,7 @@
             </a:ln>
           </c:spPr>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4292,11 +5385,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="50530666"/>
-        <c:axId val="29325947"/>
+        <c:axId val="40657352"/>
+        <c:axId val="64625165"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50530666"/>
+        <c:axId val="40657352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4312,14 +5405,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29325947"/>
+        <c:crossAx val="64625165"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29325947"/>
+        <c:axId val="64625165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4344,7 +5437,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50530666"/>
+        <c:crossAx val="40657352"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4384,15 +5477,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2016000</xdr:colOff>
+      <xdr:colOff>2070000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>288720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>853920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4405,8 +5498,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8450280" y="48600"/>
-          <a:ext cx="3836520" cy="824040"/>
+          <a:off x="8504280" y="30600"/>
+          <a:ext cx="3835800" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4421,20 +5514,155 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>58680</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>54000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>128520</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8186400" y="54000"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161280</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="25" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="91080" y="3346920"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>43920</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>20520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>120960</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="26" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="43920" y="1362240"/>
+        <a:ext cx="5766480" cy="3236040"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>109800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>5760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>186840</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>159120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="27" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="109800" y="1168200"/>
+        <a:ext cx="5766480" cy="3242160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>559800</xdr:colOff>
+      <xdr:colOff>613080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>853560</xdr:rowOff>
+      <xdr:rowOff>834840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4447,8 +5675,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10798560" y="29520"/>
-          <a:ext cx="559800" cy="824040"/>
+          <a:off x="10852560" y="11520"/>
+          <a:ext cx="559080" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4463,15 +5691,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>252360</xdr:colOff>
+      <xdr:colOff>306360</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1769040</xdr:colOff>
+      <xdr:colOff>1822320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2018880</xdr:rowOff>
+      <xdr:rowOff>2000160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4479,8 +5707,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="443880" y="1632960"/>
-        <a:ext cx="3688920" cy="1932480"/>
+        <a:off x="497880" y="1614960"/>
+        <a:ext cx="3688200" cy="1931760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4493,15 +5721,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>164160</xdr:colOff>
+      <xdr:colOff>218160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>34200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>958680</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2057040</xdr:rowOff>
+      <xdr:rowOff>2038320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4509,8 +5737,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4488480" y="1598760"/>
-        <a:ext cx="4280040" cy="2004840"/>
+        <a:off x="4542480" y="1580760"/>
+        <a:ext cx="4279320" cy="2004120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4528,15 +5756,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1006920</xdr:colOff>
+      <xdr:colOff>1060920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>561600</xdr:colOff>
+      <xdr:colOff>614880</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4549,8 +5777,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5132160" y="66600"/>
-          <a:ext cx="1727280" cy="824040"/>
+          <a:off x="5186160" y="48600"/>
+          <a:ext cx="1726560" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4565,15 +5793,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>61560</xdr:colOff>
+      <xdr:colOff>115560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>703800</xdr:colOff>
+      <xdr:colOff>757080</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>182160</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4581,8 +5809,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="253080" y="1563840"/>
-        <a:ext cx="5752080" cy="3237840"/>
+        <a:off x="307080" y="1545840"/>
+        <a:ext cx="5751360" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4595,15 +5823,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>930600</xdr:colOff>
+      <xdr:colOff>984600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>712440</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>765720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>197280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4611,8 +5839,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6231960" y="1595880"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="6285960" y="1577880"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4630,15 +5858,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>601920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4647,12 +5875,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8736840" y="96480"/>
-          <a:ext cx="4138200" cy="551520"/>
+          <a:off x="8790840" y="78480"/>
+          <a:ext cx="4137480" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4705,15 +5933,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4721,8 +5949,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2910240" y="1239480"/>
-        <a:ext cx="5816520" cy="2541240"/>
+        <a:off x="2964240" y="1221480"/>
+        <a:ext cx="5815800" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4740,15 +5968,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>601920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4757,12 +5985,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8736840" y="96480"/>
-          <a:ext cx="4138200" cy="551520"/>
+          <a:off x="8790840" y="78480"/>
+          <a:ext cx="4137480" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4815,15 +6043,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4831,8 +6059,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2910240" y="1239480"/>
-        <a:ext cx="5816520" cy="2541240"/>
+        <a:off x="2964240" y="1221480"/>
+        <a:ext cx="5815800" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4850,15 +6078,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>601920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4867,12 +6095,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8736840" y="96480"/>
-          <a:ext cx="4138200" cy="551520"/>
+          <a:off x="8790840" y="78480"/>
+          <a:ext cx="4137480" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4925,15 +6153,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4941,8 +6169,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2910240" y="1239480"/>
-        <a:ext cx="5816520" cy="2541240"/>
+        <a:off x="2964240" y="1221480"/>
+        <a:ext cx="5815800" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4960,15 +6188,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1739880</xdr:colOff>
+      <xdr:colOff>1793880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2080080</xdr:colOff>
+      <xdr:colOff>2133360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>410040</xdr:rowOff>
+      <xdr:rowOff>391320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4981,8 +6209,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1931400" y="8611560"/>
-          <a:ext cx="340200" cy="332640"/>
+          <a:off x="1985400" y="8593560"/>
+          <a:ext cx="339480" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4997,15 +6225,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1730520</xdr:colOff>
+      <xdr:colOff>1784520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2071800</xdr:colOff>
+      <xdr:colOff>2125080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>468000</xdr:rowOff>
+      <xdr:rowOff>449280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5018,8 +6246,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1922040" y="9221040"/>
-          <a:ext cx="341280" cy="333720"/>
+          <a:off x="1976040" y="9203040"/>
+          <a:ext cx="340560" cy="333000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5034,15 +6262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682560</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3948840</xdr:colOff>
+      <xdr:colOff>4002120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5051,12 +6279,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10044720" y="105840"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="10098720" y="87840"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -5109,15 +6337,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>101520</xdr:colOff>
+      <xdr:colOff>155520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>615240</xdr:colOff>
+      <xdr:colOff>668520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5130,8 +6358,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="293040" y="0"/>
-          <a:ext cx="3394800" cy="761400"/>
+          <a:off x="347040" y="0"/>
+          <a:ext cx="3394080" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5151,15 +6379,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1635120</xdr:colOff>
+      <xdr:colOff>1689120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1975320</xdr:colOff>
+      <xdr:colOff>2028600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>457560</xdr:rowOff>
+      <xdr:rowOff>438840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5172,8 +6400,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1826640" y="8573400"/>
-          <a:ext cx="340200" cy="332640"/>
+          <a:off x="1880640" y="8555400"/>
+          <a:ext cx="339480" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5188,15 +6416,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1625760</xdr:colOff>
+      <xdr:colOff>1679760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>240120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1967040</xdr:colOff>
+      <xdr:colOff>2020320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>591840</xdr:rowOff>
+      <xdr:rowOff>573120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5209,8 +6437,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1817280" y="9259200"/>
-          <a:ext cx="341280" cy="333720"/>
+          <a:off x="1871280" y="9241200"/>
+          <a:ext cx="340560" cy="333000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5225,15 +6453,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2158920</xdr:colOff>
+      <xdr:colOff>2212920</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1262880</xdr:colOff>
+      <xdr:colOff>1316160</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>3067200</xdr:rowOff>
+      <xdr:rowOff>3048480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5242,13 +6470,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="39754" t="43749" r="19608" b="14663"/>
+        <a:srcRect l="39748" t="43739" r="19603" b="14653"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2350440" y="1677240"/>
-          <a:ext cx="7242840" cy="2913840"/>
+          <a:off x="2404440" y="1659240"/>
+          <a:ext cx="7242120" cy="2913120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5263,15 +6491,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>901800</xdr:colOff>
+      <xdr:colOff>955800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4168080</xdr:colOff>
+      <xdr:colOff>4221360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5280,12 +6508,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9232200" y="96480"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="9286200" y="78480"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -5338,15 +6566,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>111240</xdr:colOff>
+      <xdr:colOff>165240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5359,8 +6587,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="302760" y="0"/>
-          <a:ext cx="3394800" cy="761400"/>
+          <a:off x="356760" y="0"/>
+          <a:ext cx="3394080" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5370,6 +6598,71 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>102240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>93960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>172440</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8713440" y="93960"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25560</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>72360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95760</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>73440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8636760" y="3604680"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -13744,6 +15037,535 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="n">
+        <v>42459</v>
+      </c>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="92"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="96"/>
+      <c r="C3" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95" t="n">
+        <f aca="false">AVERAGE(C3:I3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="97"/>
+      <c r="C4" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="95" t="n">
+        <f aca="false">AVERAGE(C4:I4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="97"/>
+      <c r="C5" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="n">
+        <f aca="false">AVERAGE(C5:I5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="98"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="95" t="e">
+        <f aca="false">AVERAGE(C6:I6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="98"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="95" t="e">
+        <f aca="false">AVERAGE(C7:I7)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="86"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="87"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="92"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="96"/>
+      <c r="C12" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="95" t="n">
+        <f aca="false">AVERAGE(C12:I12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="97"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="95" t="e">
+        <f aca="false">AVERAGE(C13:I13)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="97"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="95" t="e">
+        <f aca="false">AVERAGE(C14:I14)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="98"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="95" t="e">
+        <f aca="false">AVERAGE(C15:I15)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="98"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="95" t="e">
+        <f aca="false">AVERAGE(C16:I16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R8" activeCellId="0" sqref="R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="n">
+        <v>42459</v>
+      </c>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="92"/>
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95" t="n">
+        <f aca="false">AVERAGE(C3:I3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="99" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="94" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="95" t="n">
+        <f aca="false">AVERAGE(C4:I4)</f>
+        <v>0.6667</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="99"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="e">
+        <f aca="false">AVERAGE(C5:I5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="n">
+        <v>42459</v>
+      </c>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="92"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="99" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="99"/>
+      <c r="C3" s="94" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95" t="n">
+        <f aca="false">AVERAGE(C3:I3)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="99" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="95" t="n">
+        <f aca="false">AVERAGE(C4:I4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="99"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="e">
+        <f aca="false">AVERAGE(C5:I5)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -13751,7 +15573,7 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -17877,13 +19699,34 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+    </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
       <c r="D8" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
+      <c r="H8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="27" t="s">
@@ -17904,6 +19747,7 @@
       <c r="G9" s="27" t="s">
         <v>20</v>
       </c>
+      <c r="H9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="27" t="s">
@@ -18081,8 +19925,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -22212,7 +24056,41 @@
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
+    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+    </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
       <c r="D10" s="27" t="s">
         <v>14</v>
       </c>
@@ -30757,7 +32635,8 @@
       </c>
       <c r="D16" s="70"/>
     </row>
-    <row r="17" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="68"/>
       <c r="B17" s="69" t="s">
         <v>64</v>
       </c>
@@ -30766,14 +32645,16 @@
       </c>
       <c r="D17" s="71"/>
     </row>
-    <row r="18" s="68" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="68"/>
       <c r="B18" s="57" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="57"/>
       <c r="D18" s="57"/>
     </row>
-    <row r="19" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="68"/>
       <c r="B19" s="69" t="s">
         <v>67</v>
       </c>
@@ -30782,7 +32663,8 @@
       </c>
       <c r="D19" s="66"/>
     </row>
-    <row r="20" s="68" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="68"/>
       <c r="B20" s="69" t="s">
         <v>69</v>
       </c>
@@ -30791,7 +32673,8 @@
       </c>
       <c r="D20" s="72"/>
     </row>
-    <row r="21" s="68" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="68"/>
       <c r="B21" s="69" t="s">
         <v>71</v>
       </c>
@@ -30800,21 +32683,24 @@
       </c>
       <c r="D21" s="70"/>
     </row>
-    <row r="22" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="68"/>
       <c r="B22" s="73" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
     </row>
-    <row r="23" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="68"/>
       <c r="B23" s="74" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="74"/>
       <c r="D23" s="74"/>
     </row>
-    <row r="24" s="68" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="68"/>
       <c r="B24" s="69" t="s">
         <v>74</v>
       </c>
@@ -37157,7 +39043,8 @@
       </c>
       <c r="D16" s="82"/>
     </row>
-    <row r="17" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="68"/>
       <c r="B17" s="81" t="s">
         <v>64</v>
       </c>
@@ -37166,14 +39053,16 @@
       </c>
       <c r="D17" s="71"/>
     </row>
-    <row r="18" s="68" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="68"/>
       <c r="B18" s="78" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="78"/>
       <c r="D18" s="78"/>
     </row>
-    <row r="19" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="68"/>
       <c r="B19" s="81" t="s">
         <v>67</v>
       </c>
@@ -37182,7 +39071,8 @@
       </c>
       <c r="D19" s="66"/>
     </row>
-    <row r="20" s="68" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="68"/>
       <c r="B20" s="81" t="s">
         <v>69</v>
       </c>
@@ -37191,7 +39081,8 @@
       </c>
       <c r="D20" s="72"/>
     </row>
-    <row r="21" s="68" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="68"/>
       <c r="B21" s="81" t="s">
         <v>71</v>
       </c>
@@ -37200,21 +39091,24 @@
       </c>
       <c r="D21" s="70"/>
     </row>
-    <row r="22" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="68"/>
       <c r="B22" s="83" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="83"/>
       <c r="D22" s="83"/>
     </row>
-    <row r="23" s="68" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="68"/>
       <c r="B23" s="84" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="84"/>
       <c r="D23" s="84"/>
     </row>
-    <row r="24" s="68" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="68"/>
       <c r="B24" s="75" t="s">
         <v>74</v>
       </c>
@@ -37299,4 +39193,322 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="89" t="n">
+        <v>42459</v>
+      </c>
+      <c r="D2" s="90" t="n">
+        <v>42475</v>
+      </c>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="92"/>
+    </row>
+    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95" t="n">
+        <f aca="false">AVERAGE(C3:I3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="93" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="93"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="95" t="n">
+        <f aca="false">AVERAGE(C4:I4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="D5" s="94" t="n">
+        <v>0.9091</v>
+      </c>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="n">
+        <f aca="false">AVERAGE(C5:I5)</f>
+        <v>0.89205</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="93"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="95" t="n">
+        <f aca="false">AVERAGE(C6:I6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="95" t="n">
+        <f aca="false">AVERAGE(C7:I7)</f>
+        <v>0.6667</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="93"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="95" t="e">
+        <f aca="false">AVERAGE(C8:I8)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="95" t="e">
+        <f aca="false">AVERAGE(C9:I9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="86"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="88" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="87"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
+      <c r="F17" s="91"/>
+      <c r="G17" s="91"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="91"/>
+      <c r="J17" s="92"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="96" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="96"/>
+      <c r="C18" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="95" t="n">
+        <f aca="false">AVERAGE(C18:I18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="96"/>
+      <c r="C19" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="95" t="n">
+        <f aca="false">AVERAGE(C19:I19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="96"/>
+      <c r="C20" s="94" t="n">
+        <v>0.8889</v>
+      </c>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="95" t="n">
+        <f aca="false">AVERAGE(C20:I20)</f>
+        <v>0.8889</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="96"/>
+      <c r="C21" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="94"/>
+      <c r="H21" s="94"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="95" t="n">
+        <f aca="false">AVERAGE(C21:I21)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
actualización concentrdo de métricas
</commit_message>
<xml_diff>
--- a/Organizacional/06. Medición y Monitoreo/2016/Bisoltec-ConcentradoMetricas.xlsx
+++ b/Organizacional/06. Medición y Monitoreo/2016/Bisoltec-ConcentradoMetricas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ObjetivosNegocio" sheetId="1" state="visible" r:id="rId2"/>
@@ -927,7 +927,7 @@
     <numFmt numFmtId="165" formatCode="[$$-80A]#,##0.00;[RED]\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1037,6 +1037,11 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
@@ -1119,7 +1124,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF420E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1573,7 +1578,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1581,11 +1586,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1641,11 +1646,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1673,7 +1678,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1681,27 +1686,27 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1709,27 +1714,27 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1745,7 +1750,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1753,19 +1758,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1825,7 +1830,7 @@
       <rgbColor rgb="FF9BBB59"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FFA6A6A6"/>
       <rgbColor rgb="FF004586"/>
@@ -1947,11 +1952,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="25219919"/>
-        <c:axId val="20082621"/>
+        <c:axId val="72519183"/>
+        <c:axId val="94353003"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25219919"/>
+        <c:axId val="72519183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,14 +1972,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20082621"/>
+        <c:crossAx val="94353003"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20082621"/>
+        <c:axId val="94353003"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2004,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="25219919"/>
+        <c:crossAx val="72519183"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2140,11 +2145,11 @@
           <c:downBars/>
         </c:upDownBars>
         <c:marker val="1"/>
-        <c:axId val="98400373"/>
-        <c:axId val="22943621"/>
+        <c:axId val="50225048"/>
+        <c:axId val="98053143"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98400373"/>
+        <c:axId val="50225048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,14 +2165,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22943621"/>
+        <c:crossAx val="98053143"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22943621"/>
+        <c:axId val="98053143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2197,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="98400373"/>
+        <c:crossAx val="50225048"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2228,6 +2233,506 @@
 </file>
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Control de Gastos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado (Horas)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de esfuerzo'!$D$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real (Horas)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de esfuerzo'!$D$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="81180761"/>
+        <c:axId val="46114164"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="81180761"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="46114164"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="46114164"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="81180761"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado (Horas)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de esfuerzo'!$D$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real (Horas)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de esfuerzo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de esfuerzo'!$D$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="24971086"/>
+        <c:axId val="1772292"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="24971086"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="1772292"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1772292"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="24971086"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2310,11 +2815,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="57148263"/>
-        <c:axId val="79509559"/>
+        <c:axId val="77522723"/>
+        <c:axId val="68713541"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57148263"/>
+        <c:axId val="77522723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,14 +2835,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79509559"/>
+        <c:crossAx val="68713541"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79509559"/>
+        <c:axId val="68713541"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,7 +2867,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57148263"/>
+        <c:crossAx val="77522723"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2397,7 +2902,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2480,11 +2985,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="13143594"/>
-        <c:axId val="30676547"/>
+        <c:axId val="38880640"/>
+        <c:axId val="23183248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="13143594"/>
+        <c:axId val="38880640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2500,14 +3005,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30676547"/>
+        <c:crossAx val="23183248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30676547"/>
+        <c:axId val="23183248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2532,7 +3037,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13143594"/>
+        <c:crossAx val="38880640"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2567,7 +3072,491 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de Costo'!$D$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de Costo'!$D$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>468.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="2130792"/>
+        <c:axId val="74007872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2130792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="74007872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="74007872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2130792"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planeado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de Costo'!$D$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5573</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desviación de Costo'!$D$8:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Requerimientos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Planeación</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Desarrollo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Entrega</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviación de Costo'!$D$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="50658806"/>
+        <c:axId val="14057303"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50658806"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="14057303"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="14057303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="50658806"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3004,11 +3993,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="92504728"/>
-        <c:axId val="10984637"/>
+        <c:axId val="73110970"/>
+        <c:axId val="10417427"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92504728"/>
+        <c:axId val="73110970"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,14 +4014,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10984637"/>
+        <c:crossAx val="10417427"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10984637"/>
+        <c:axId val="10417427"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3058,7 +4047,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92504728"/>
+        <c:crossAx val="73110970"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="20"/>
       </c:valAx>
@@ -3097,7 +4086,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3534,11 +4523,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="82294555"/>
-        <c:axId val="27197393"/>
+        <c:axId val="65400472"/>
+        <c:axId val="89850340"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82294555"/>
+        <c:axId val="65400472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3555,14 +4544,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27197393"/>
+        <c:crossAx val="89850340"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27197393"/>
+        <c:axId val="89850340"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3588,7 +4577,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82294555"/>
+        <c:crossAx val="65400472"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="20"/>
       </c:valAx>
@@ -3627,7 +4616,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4064,11 +5053,11 @@
         </c:ser>
         <c:gapWidth val="65"/>
         <c:overlap val="0"/>
-        <c:axId val="47353836"/>
-        <c:axId val="53904605"/>
+        <c:axId val="93067497"/>
+        <c:axId val="91596329"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47353836"/>
+        <c:axId val="93067497"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4085,14 +5074,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53904605"/>
+        <c:crossAx val="91596329"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53904605"/>
+        <c:axId val="91596329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -4118,7 +5107,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47353836"/>
+        <c:crossAx val="93067497"/>
         <c:crosses val="autoZero"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
@@ -4163,15 +5152,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2016000</xdr:colOff>
+      <xdr:colOff>2070000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>288720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>853920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4184,8 +5173,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8532360" y="48600"/>
-          <a:ext cx="3910320" cy="824040"/>
+          <a:off x="8586360" y="30600"/>
+          <a:ext cx="3909600" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4205,15 +5194,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88920</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>119160</xdr:colOff>
+      <xdr:colOff>172440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>853560</xdr:rowOff>
+      <xdr:rowOff>834840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4226,110 +5215,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9399240" y="29520"/>
-          <a:ext cx="3255840" cy="824040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1995120</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2781720</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="267480" y="1658880"/>
-        <a:ext cx="5081040" cy="2703960"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2963880</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>246600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>942120</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2664000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="6317280" y="1827720"/>
-        <a:ext cx="5179680" cy="2417400"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>177840</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1018800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="2 Imagen" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="380880" y="95400"/>
-          <a:ext cx="3038760" cy="824040"/>
+          <a:off x="9453240" y="11520"/>
+          <a:ext cx="3255120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4344,24 +5231,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>282240</xdr:colOff>
+      <xdr:colOff>4320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>295560</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1091160</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2048400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2437200</xdr:rowOff>
+      <xdr:rowOff>2763000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="2" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="485280" y="1781280"/>
-        <a:ext cx="5204520" cy="2141640"/>
+        <a:off x="321480" y="1640880"/>
+        <a:ext cx="5080320" cy="2703240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4373,29 +5260,251 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1510920</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>197280</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11160</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2621160</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2153880</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvPr id="3" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6109560" y="1683000"/>
-        <a:ext cx="4879440" cy="2423880"/>
+        <a:off x="328320" y="7020360"/>
+        <a:ext cx="5178960" cy="2416680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2610720</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>100440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>126360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5964120" y="7084800"/>
+        <a:ext cx="4691160" cy="2330640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3134520</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>27360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533160</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2807640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6487920" y="1608480"/>
+        <a:ext cx="4600080" cy="2780280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>231840</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1072080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="2 Imagen" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="434880" y="77400"/>
+          <a:ext cx="3038040" cy="823320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>336240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>277560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1144440</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2418480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="539280" y="1763280"/>
+        <a:ext cx="5203800" cy="2140920"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>128520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>611640</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>22680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="331560" y="6561000"/>
+        <a:ext cx="4878720" cy="2423160"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1308240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1936080</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2786040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5906880" y="1610280"/>
+        <a:ext cx="4553280" cy="2661480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1569960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>111960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2238120</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>34200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6168600" y="6977880"/>
+        <a:ext cx="4593600" cy="2227320"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4409,29 +5518,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3901320</xdr:colOff>
+      <xdr:colOff>3954600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvPr id="11" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8853840" y="96480"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="8907840" y="78480"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4484,24 +5593,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Gráfico 2"/>
+        <xdr:cNvPr id="12" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2947320" y="1239480"/>
-        <a:ext cx="5896440" cy="2541240"/>
+        <a:off x="3001320" y="1221480"/>
+        <a:ext cx="5895720" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4519,29 +5628,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3901320</xdr:colOff>
+      <xdr:colOff>3954600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvPr id="13" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8853840" y="96480"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="8907840" y="78480"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4594,24 +5703,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Gráfico 2"/>
+        <xdr:cNvPr id="14" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2947320" y="1239480"/>
-        <a:ext cx="5896440" cy="2541240"/>
+        <a:off x="3001320" y="1221480"/>
+        <a:ext cx="5895720" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4629,29 +5738,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>689040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3901320</xdr:colOff>
+      <xdr:colOff>3954600</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="CustomShape 1"/>
+        <xdr:cNvPr id="15" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8853840" y="96480"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="8907840" y="78480"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4704,24 +5813,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>546480</xdr:colOff>
+      <xdr:colOff>600480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2637720</xdr:rowOff>
+      <xdr:rowOff>2619000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Gráfico 2"/>
+        <xdr:cNvPr id="16" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2947320" y="1239480"/>
-        <a:ext cx="5896440" cy="2541240"/>
+        <a:off x="3001320" y="1221480"/>
+        <a:ext cx="5895720" cy="2540520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4739,19 +5848,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1739880</xdr:colOff>
+      <xdr:colOff>1793880</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2080080</xdr:colOff>
+      <xdr:colOff>2133360</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>410040</xdr:rowOff>
+      <xdr:rowOff>391320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Imagen 3" descr=""/>
+        <xdr:cNvPr id="17" name="Imagen 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4760,8 +5869,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1942920" y="8611560"/>
-          <a:ext cx="340200" cy="332640"/>
+          <a:off x="1996920" y="8593560"/>
+          <a:ext cx="339480" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4776,19 +5885,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1730520</xdr:colOff>
+      <xdr:colOff>1784520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2071800</xdr:colOff>
+      <xdr:colOff>2125080</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>468000</xdr:rowOff>
+      <xdr:rowOff>449280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Imagen 4" descr=""/>
+        <xdr:cNvPr id="18" name="Imagen 4" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4797,8 +5906,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1933560" y="9221040"/>
-          <a:ext cx="341280" cy="333720"/>
+          <a:off x="1987560" y="9203040"/>
+          <a:ext cx="340560" cy="333000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4813,29 +5922,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>682560</xdr:colOff>
+      <xdr:colOff>736560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3948840</xdr:colOff>
+      <xdr:colOff>4002120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>67320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvPr id="19" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10171080" y="105840"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="10225080" y="87840"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -4888,19 +5997,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>101520</xdr:colOff>
+      <xdr:colOff>155520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>615240</xdr:colOff>
+      <xdr:colOff>668520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="6 Imagen" descr=""/>
+        <xdr:cNvPr id="20" name="6 Imagen" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4909,8 +6018,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304560" y="0"/>
-          <a:ext cx="3435480" cy="761400"/>
+          <a:off x="358560" y="0"/>
+          <a:ext cx="3434760" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4930,19 +6039,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1635120</xdr:colOff>
+      <xdr:colOff>1689120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1975320</xdr:colOff>
+      <xdr:colOff>2028600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>457560</xdr:rowOff>
+      <xdr:rowOff>438840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Imagen 1" descr=""/>
+        <xdr:cNvPr id="21" name="Imagen 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4951,8 +6060,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1838160" y="8573400"/>
-          <a:ext cx="340200" cy="332640"/>
+          <a:off x="1892160" y="8555400"/>
+          <a:ext cx="339480" cy="331920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4967,19 +6076,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1625760</xdr:colOff>
+      <xdr:colOff>1679760</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>258120</xdr:rowOff>
+      <xdr:rowOff>240120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1967040</xdr:colOff>
+      <xdr:colOff>2020320</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>591840</xdr:rowOff>
+      <xdr:rowOff>573120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Imagen 2" descr=""/>
+        <xdr:cNvPr id="22" name="Imagen 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4988,8 +6097,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1828800" y="9259200"/>
-          <a:ext cx="341280" cy="333720"/>
+          <a:off x="1882800" y="9241200"/>
+          <a:ext cx="340560" cy="333000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5004,30 +6113,30 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2158920</xdr:colOff>
+      <xdr:colOff>2212920</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1262880</xdr:colOff>
+      <xdr:colOff>1316160</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>3067200</xdr:rowOff>
+      <xdr:rowOff>3048480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Imagen 3" descr=""/>
+        <xdr:cNvPr id="23" name="Imagen 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="39751" t="43749" r="19605" b="14653"/>
+        <a:srcRect l="39745" t="43739" r="19600" b="14643"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2361960" y="1677240"/>
-          <a:ext cx="7347600" cy="2913840"/>
+          <a:off x="2415960" y="1659240"/>
+          <a:ext cx="7346880" cy="2913120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5042,29 +6151,29 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>901800</xdr:colOff>
+      <xdr:colOff>955800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4168080</xdr:colOff>
+      <xdr:colOff>4221360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="CustomShape 1"/>
+        <xdr:cNvPr id="24" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9348480" y="96480"/>
-          <a:ext cx="3266280" cy="551520"/>
+          <a:off x="9402480" y="78480"/>
+          <a:ext cx="3265560" cy="550800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 14400"/>
+            <a:gd name="adj" fmla="val 13805"/>
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
@@ -5117,19 +6226,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>111240</xdr:colOff>
+      <xdr:colOff>165240</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>624960</xdr:colOff>
+      <xdr:colOff>678240</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="5 Imagen" descr=""/>
+        <xdr:cNvPr id="25" name="5 Imagen" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -5138,8 +6247,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314280" y="0"/>
-          <a:ext cx="3435480" cy="761400"/>
+          <a:off x="368280" y="0"/>
+          <a:ext cx="3434760" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13530,8 +14639,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -22945,8 +24054,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -35676,7 +36785,8 @@
       </c>
       <c r="D16" s="75"/>
     </row>
-    <row r="17" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="73"/>
       <c r="B17" s="74" t="s">
         <v>62</v>
       </c>
@@ -35685,14 +36795,16 @@
       </c>
       <c r="D17" s="76"/>
     </row>
-    <row r="18" s="73" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="73"/>
       <c r="B18" s="62" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="62"/>
       <c r="D18" s="62"/>
     </row>
-    <row r="19" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="73"/>
       <c r="B19" s="74" t="s">
         <v>65</v>
       </c>
@@ -35701,7 +36813,8 @@
       </c>
       <c r="D19" s="71"/>
     </row>
-    <row r="20" s="73" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="73"/>
       <c r="B20" s="74" t="s">
         <v>67</v>
       </c>
@@ -35710,7 +36823,8 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" s="73" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="73"/>
       <c r="B21" s="74" t="s">
         <v>69</v>
       </c>
@@ -35719,21 +36833,24 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="73"/>
       <c r="B22" s="59" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
     </row>
-    <row r="23" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="73"/>
       <c r="B23" s="77" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="77"/>
       <c r="D23" s="77"/>
     </row>
-    <row r="24" s="73" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="73"/>
       <c r="B24" s="74" t="s">
         <v>72</v>
       </c>
@@ -42076,7 +43193,8 @@
       </c>
       <c r="D16" s="85"/>
     </row>
-    <row r="17" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="73"/>
       <c r="B17" s="84" t="s">
         <v>62</v>
       </c>
@@ -42085,14 +43203,16 @@
       </c>
       <c r="D17" s="76"/>
     </row>
-    <row r="18" s="73" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="73"/>
       <c r="B18" s="81" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="81"/>
       <c r="D18" s="81"/>
     </row>
-    <row r="19" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="73"/>
       <c r="B19" s="84" t="s">
         <v>65</v>
       </c>
@@ -42101,7 +43221,8 @@
       </c>
       <c r="D19" s="71"/>
     </row>
-    <row r="20" s="73" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="73"/>
       <c r="B20" s="84" t="s">
         <v>67</v>
       </c>
@@ -42110,7 +43231,8 @@
       </c>
       <c r="D20" s="75"/>
     </row>
-    <row r="21" s="73" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="73"/>
       <c r="B21" s="84" t="s">
         <v>69</v>
       </c>
@@ -42119,21 +43241,24 @@
       </c>
       <c r="D21" s="75"/>
     </row>
-    <row r="22" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="73"/>
       <c r="B22" s="79" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="79"/>
       <c r="D22" s="79"/>
     </row>
-    <row r="23" s="73" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="73"/>
       <c r="B23" s="86" t="s">
         <v>71</v>
       </c>
       <c r="C23" s="86"/>
       <c r="D23" s="86"/>
     </row>
-    <row r="24" s="73" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="73"/>
       <c r="B24" s="78" t="s">
         <v>72</v>
       </c>

</xml_diff>